<commit_message>
0.1.04 - Change algorithm for double nodes function
</commit_message>
<xml_diff>
--- a/Source/Excel/Test/SpeedTest.xlsx
+++ b/Source/Excel/Test/SpeedTest.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>Divide Member</t>
   </si>
@@ -34,12 +34,21 @@
   <si>
     <t>Upload member</t>
   </si>
+  <si>
+    <t>Algo 1</t>
+  </si>
+  <si>
+    <t>Algo 2</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -48,16 +57,51 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -65,13 +109,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -197,7 +272,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Лист1!$B$3:$B$9</c:f>
+              <c:f>Лист1!$B$4:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -227,7 +302,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Лист1!$C$3:$C$9</c:f>
+              <c:f>Лист1!$C$4:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -250,7 +325,7 @@
                   <c:v>913.178</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -265,11 +340,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="223877040"/>
-        <c:axId val="223878160"/>
+        <c:axId val="221828896"/>
+        <c:axId val="221830016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="223877040"/>
+        <c:axId val="221828896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -326,12 +401,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223878160"/>
+        <c:crossAx val="221830016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="223878160"/>
+        <c:axId val="221830016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -388,7 +463,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223877040"/>
+        <c:crossAx val="221828896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -515,12 +590,15 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Algo2</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -531,11 +609,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -543,7 +621,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Лист1!$E$3:$E$9</c:f>
+              <c:f>Лист1!$F$4:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -573,30 +651,30 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Лист1!$F$3:$F$9</c:f>
+              <c:f>Лист1!$H$4:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2.8000000000000001E-2</c:v>
+                  <c:v>1.2E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.75</c:v>
+                  <c:v>0.111</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.07</c:v>
+                  <c:v>0.22600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44.34</c:v>
+                  <c:v>0.55100000000000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>103.06</c:v>
+                  <c:v>0.83299999999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>175.75</c:v>
+                  <c:v>1.157</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>2.33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -611,11 +689,121 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="228325296"/>
-        <c:axId val="228324736"/>
+        <c:axId val="222205904"/>
+        <c:axId val="222206464"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:v>Algo1</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Лист1!$F$4:$F$10</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>200</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>400</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1000</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1500</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2000</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>4000</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Лист1!$G$4:$G$10</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>2.8000000000000001E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.75</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>7.07</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>44.34</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>103.06</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>175.75</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>350</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="1"/>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="228325296"/>
+        <c:axId val="222205904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -672,12 +860,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228324736"/>
+        <c:crossAx val="222206464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="228324736"/>
+        <c:axId val="222206464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -734,7 +922,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228325296"/>
+        <c:crossAx val="222205904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -889,7 +1077,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Лист1!$H$3:$H$9</c:f>
+              <c:f>Лист1!$J$4:$J$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -919,7 +1107,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Лист1!$I$3:$I$9</c:f>
+              <c:f>Лист1!$K$4:$K$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -942,7 +1130,7 @@
                   <c:v>37.234999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>132.88300000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -957,11 +1145,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="228330336"/>
-        <c:axId val="228327536"/>
+        <c:axId val="222208704"/>
+        <c:axId val="222209264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="228330336"/>
+        <c:axId val="222208704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1018,12 +1206,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228327536"/>
+        <c:crossAx val="222209264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="228327536"/>
+        <c:axId val="222209264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1080,7 +1268,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228330336"/>
+        <c:crossAx val="222208704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2803,13 +2991,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2831,15 +3019,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2861,15 +3049,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3155,175 +3343,248 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I9"/>
+  <dimension ref="B2:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="4" width="9.140625" style="1"/>
+    <col min="7" max="8" width="9.140625" style="1"/>
+    <col min="11" max="12" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="E2" s="1" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="F2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="J2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="1"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="4">
         <v>10</v>
       </c>
-      <c r="C3">
+      <c r="C4" s="5">
         <v>0.10199999999999999</v>
       </c>
-      <c r="E3">
+      <c r="D4" s="5"/>
+      <c r="F4" s="4">
         <v>20</v>
       </c>
-      <c r="F3">
+      <c r="G4" s="5">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="H3">
+      <c r="H4" s="5">
+        <v>1.2E-2</v>
+      </c>
+      <c r="J4" s="4">
         <v>10</v>
       </c>
-      <c r="I3">
+      <c r="K4" s="5">
         <v>0.52200000000000002</v>
       </c>
+      <c r="L4" s="5"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="4">
         <v>100</v>
       </c>
-      <c r="C4">
+      <c r="C5" s="5">
         <v>8.77</v>
       </c>
-      <c r="E4">
+      <c r="D5" s="5"/>
+      <c r="F5" s="4">
         <v>200</v>
       </c>
-      <c r="F4">
+      <c r="G5" s="5">
         <v>1.75</v>
       </c>
-      <c r="H4">
+      <c r="H5" s="5">
+        <v>0.111</v>
+      </c>
+      <c r="J5" s="4">
         <v>100</v>
       </c>
-      <c r="I4">
+      <c r="K5" s="5">
         <v>3.6160000000000001</v>
       </c>
+      <c r="L5" s="5"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
         <v>200</v>
       </c>
-      <c r="C5">
+      <c r="C6" s="5">
         <v>35.47</v>
       </c>
-      <c r="E5">
+      <c r="D6" s="5"/>
+      <c r="F6" s="4">
         <v>400</v>
       </c>
-      <c r="F5">
+      <c r="G6" s="5">
         <v>7.07</v>
       </c>
-      <c r="H5">
+      <c r="H6" s="5">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="J6" s="4">
         <v>200</v>
       </c>
-      <c r="I5">
+      <c r="K6" s="5">
         <v>7.14</v>
       </c>
+      <c r="L6" s="5"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="4">
         <v>500</v>
       </c>
-      <c r="C6">
+      <c r="C7" s="5">
         <v>225.76</v>
       </c>
-      <c r="E6">
+      <c r="D7" s="5"/>
+      <c r="F7" s="4">
         <v>1000</v>
       </c>
-      <c r="F6">
+      <c r="G7" s="5">
         <v>44.34</v>
       </c>
-      <c r="H6">
+      <c r="H7" s="5">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="J7" s="4">
         <v>500</v>
       </c>
-      <c r="I6">
+      <c r="K7" s="5">
         <v>18.2</v>
       </c>
+      <c r="L7" s="5"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="4">
         <v>750</v>
       </c>
-      <c r="C7">
+      <c r="C8" s="5">
         <v>498.61</v>
       </c>
-      <c r="E7">
+      <c r="D8" s="5"/>
+      <c r="F8" s="4">
         <v>1500</v>
       </c>
-      <c r="F7">
+      <c r="G8" s="5">
         <v>103.06</v>
       </c>
-      <c r="H7">
+      <c r="H8" s="5">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="J8" s="4">
         <v>750</v>
       </c>
-      <c r="I7">
+      <c r="K8" s="5">
         <v>28.49</v>
       </c>
+      <c r="L8" s="5"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
         <v>1000</v>
       </c>
-      <c r="C8">
+      <c r="C9" s="5">
         <v>913.178</v>
       </c>
-      <c r="E8">
+      <c r="D9" s="5"/>
+      <c r="F9" s="4">
         <v>2000</v>
       </c>
-      <c r="F8">
+      <c r="G9" s="5">
         <v>175.75</v>
       </c>
-      <c r="H8">
+      <c r="H9" s="5">
+        <v>1.157</v>
+      </c>
+      <c r="J9" s="4">
         <v>1000</v>
       </c>
-      <c r="I8">
+      <c r="K9" s="5">
         <v>37.234999999999999</v>
       </c>
+      <c r="L9" s="5"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
         <v>2000</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="E9">
+      <c r="C10" s="7">
+        <v>2000</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="F10" s="4">
         <v>4000</v>
       </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="H9">
+      <c r="G10" s="7">
+        <v>350</v>
+      </c>
+      <c r="H10" s="5">
+        <v>2.33</v>
+      </c>
+      <c r="J10" s="4">
         <v>2000</v>
       </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
+      <c r="K10" s="5">
+        <v>132.88300000000001</v>
+      </c>
+      <c r="L10" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="B2:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
0.1.06 - Change algorithm for double nodes
</commit_message>
<xml_diff>
--- a/Source/Excel/Test/SpeedTest.xlsx
+++ b/Source/Excel/Test/SpeedTest.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
   <si>
     <t>Divide Member</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>Count</t>
+  </si>
+  <si>
+    <t>Algo 3</t>
   </si>
 </sst>
 </file>
@@ -101,7 +104,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -124,11 +127,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -147,6 +170,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -340,11 +369,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="208617264"/>
-        <c:axId val="208617824"/>
+        <c:axId val="224625008"/>
+        <c:axId val="224626128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="208617264"/>
+        <c:axId val="224625008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -401,12 +430,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208617824"/>
+        <c:crossAx val="224626128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="208617824"/>
+        <c:axId val="224626128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -463,7 +492,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208617264"/>
+        <c:crossAx val="224625008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -689,8 +718,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="208620624"/>
-        <c:axId val="208621184"/>
+        <c:axId val="226229776"/>
+        <c:axId val="226230336"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -803,7 +832,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="208620624"/>
+        <c:axId val="226229776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -860,12 +889,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208621184"/>
+        <c:crossAx val="226230336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="208621184"/>
+        <c:axId val="226230336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -922,7 +951,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208620624"/>
+        <c:crossAx val="226229776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1077,7 +1106,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Лист1!$J$4:$J$10</c:f>
+              <c:f>Лист1!$K$4:$K$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1107,7 +1136,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Лист1!$K$4:$K$10</c:f>
+              <c:f>Лист1!$L$4:$L$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1145,11 +1174,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="208623424"/>
-        <c:axId val="210584144"/>
+        <c:axId val="226232576"/>
+        <c:axId val="226233136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="208623424"/>
+        <c:axId val="226232576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1206,12 +1235,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210584144"/>
+        <c:crossAx val="226233136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="210584144"/>
+        <c:axId val="226233136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1268,7 +1297,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208623424"/>
+        <c:crossAx val="226232576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2995,7 +3024,7 @@
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
@@ -3019,13 +3048,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -3049,13 +3078,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>295275</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
@@ -3343,37 +3372,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L10"/>
+  <dimension ref="B2:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="4" width="9.140625" style="1"/>
-    <col min="7" max="8" width="9.140625" style="1"/>
-    <col min="11" max="12" width="9.140625" style="1"/>
+    <col min="7" max="9" width="9.140625" style="1"/>
+    <col min="12" max="13" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="J2" s="7" t="s">
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="K2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="7"/>
       <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
@@ -3392,17 +3422,20 @@
       <c r="H3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="I3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>10</v>
       </c>
@@ -3421,15 +3454,18 @@
       <c r="H4" s="4">
         <v>1.2E-2</v>
       </c>
-      <c r="J4" s="3">
+      <c r="I4" s="4">
+        <v>5.5E-2</v>
+      </c>
+      <c r="K4" s="3">
         <v>10</v>
       </c>
-      <c r="K4" s="4">
+      <c r="L4" s="4">
         <v>0.52200000000000002</v>
       </c>
-      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>100</v>
       </c>
@@ -3448,15 +3484,18 @@
       <c r="H5" s="4">
         <v>0.111</v>
       </c>
-      <c r="J5" s="3">
+      <c r="I5" s="4">
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="K5" s="3">
         <v>100</v>
       </c>
-      <c r="K5" s="4">
+      <c r="L5" s="4">
         <v>3.6160000000000001</v>
       </c>
-      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>200</v>
       </c>
@@ -3475,15 +3514,18 @@
       <c r="H6" s="4">
         <v>0.22600000000000001</v>
       </c>
-      <c r="J6" s="3">
+      <c r="I6" s="4">
+        <v>2.4580000000000002</v>
+      </c>
+      <c r="K6" s="3">
         <v>200</v>
       </c>
-      <c r="K6" s="4">
+      <c r="L6" s="4">
         <v>7.14</v>
       </c>
-      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>500</v>
       </c>
@@ -3502,15 +3544,18 @@
       <c r="H7" s="4">
         <v>0.55100000000000005</v>
       </c>
-      <c r="J7" s="3">
+      <c r="I7" s="4">
+        <v>6.0190000000000001</v>
+      </c>
+      <c r="K7" s="3">
         <v>500</v>
       </c>
-      <c r="K7" s="4">
+      <c r="L7" s="4">
         <v>18.2</v>
       </c>
-      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>750</v>
       </c>
@@ -3529,15 +3574,18 @@
       <c r="H8" s="4">
         <v>0.83299999999999996</v>
       </c>
-      <c r="J8" s="3">
+      <c r="I8" s="4">
+        <v>10.397</v>
+      </c>
+      <c r="K8" s="3">
         <v>750</v>
       </c>
-      <c r="K8" s="4">
+      <c r="L8" s="4">
         <v>28.49</v>
       </c>
-      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <v>1000</v>
       </c>
@@ -3556,15 +3604,18 @@
       <c r="H9" s="4">
         <v>1.157</v>
       </c>
-      <c r="J9" s="3">
+      <c r="I9" s="4">
+        <v>13.468999999999999</v>
+      </c>
+      <c r="K9" s="3">
         <v>1000</v>
       </c>
-      <c r="K9" s="4">
+      <c r="L9" s="4">
         <v>37.234999999999999</v>
       </c>
-      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>2000</v>
       </c>
@@ -3583,19 +3634,20 @@
       <c r="H10" s="4">
         <v>2.33</v>
       </c>
-      <c r="J10" s="3">
+      <c r="I10" s="4"/>
+      <c r="K10" s="3">
         <v>2000</v>
       </c>
-      <c r="K10" s="4">
+      <c r="L10" s="4">
         <v>68.718999999999994</v>
       </c>
-      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="K2:M2"/>
     <mergeCell ref="B2:D2"/>
+    <mergeCell ref="F2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>

</xml_diff>